<commit_message>
modified:   data/events.xlsx 	modified:   src/app_ald_TMA.cpp
</commit_message>
<xml_diff>
--- a/data/events.xlsx
+++ b/data/events.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="48">
   <si>
     <t>type</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>OAlb</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1324,7 @@
   <dimension ref="A1:K769"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="I133" sqref="I133"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1679,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <v>0.791</v>
+        <v>1.13</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>16</v>
@@ -1705,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>0.791</v>
+        <v>1.13</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>18</v>
@@ -1731,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <v>0.791</v>
+        <v>1.13</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>28</v>
@@ -2797,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2">
-        <v>0.791</v>
+        <v>1.13</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>16</v>
@@ -2823,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="2">
-        <v>0.791</v>
+        <v>1.13</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>18</v>
@@ -2849,7 +2852,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="2">
-        <v>0.791</v>
+        <v>1.13</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>28</v>
@@ -5245,7 +5248,9 @@
     <row r="133" spans="7:10">
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
-      <c r="I133" s="2"/>
+      <c r="I133" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="J133" s="2"/>
     </row>
     <row r="134" spans="7:10">

</xml_diff>